<commit_message>
Updated the sheet with sprint plan and project requirements
Updated the sheet with sprint plan and project requirements
</commit_message>
<xml_diff>
--- a/ProjectDocuments/P3-USF-iOSBatch-Project - HandBook.xlsx
+++ b/ProjectDocuments/P3-USF-iOSBatch-Project - HandBook.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KLST\Revature\USF\iOS\Projects\P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4400A8-2E7E-4F2B-B179-20570BA016F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BC263B-BE8C-431C-89F9-793F01EEF607}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B7BEAE90-68F9-4A87-9D57-B62586C9BC90}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="6" r:id="rId1"/>
-    <sheet name="Course &amp; Quiz Management" sheetId="1" r:id="rId2"/>
+    <sheet name="iRevatureQuizPro" sheetId="1" r:id="rId2"/>
     <sheet name="Sprint Plan" sheetId="2" r:id="rId3"/>
     <sheet name="Project Resources" sheetId="3" r:id="rId4"/>
     <sheet name="Tasks - Owners" sheetId="4" r:id="rId5"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="127">
   <si>
     <t>User Story</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Event</t>
   </si>
   <si>
-    <t>As a revature ambassdor I should be able to attach a quiz to an event code (sent from Marketo)</t>
-  </si>
-  <si>
     <t>As a event Attendee I should be able to enter into an event and takeup quiz</t>
   </si>
   <si>
@@ -323,9 +320,6 @@
     <t>04-Mar - 2pm (Uday) - 05th Mar</t>
   </si>
   <si>
-    <t>As a Trainer I should be able to import questions</t>
-  </si>
-  <si>
     <t>Actual</t>
   </si>
   <si>
@@ -338,18 +332,12 @@
     <t>Description</t>
   </si>
   <si>
-    <t>This project is a iOS Mobile App which enables trainers, ambassadors and associates to configure/access the quiz</t>
-  </si>
-  <si>
     <t>iOS USF Batch - JAN 2020</t>
   </si>
   <si>
     <t>Project Type</t>
   </si>
   <si>
-    <t>P3 Project</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -366,13 +354,76 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Trainer I should be able to import questions </t>
+  </si>
+  <si>
+    <t>Total User Stories</t>
+  </si>
+  <si>
+    <t>GitHub Location</t>
+  </si>
+  <si>
+    <t>https://github.com/revaturelabs/iRevatureQuizPro/</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Xcode</t>
+  </si>
+  <si>
+    <t>iOS</t>
+  </si>
+  <si>
+    <t>Swift</t>
+  </si>
+  <si>
+    <t>MacOS</t>
+  </si>
+  <si>
+    <t>Alamofire</t>
+  </si>
+  <si>
+    <t>SwiftyJSON</t>
+  </si>
+  <si>
+    <t>SQLite Framework</t>
+  </si>
+  <si>
+    <t>Postman</t>
+  </si>
+  <si>
+    <t>MySQL - Server Side</t>
+  </si>
+  <si>
+    <t>GCP Cloud - Kubernetes</t>
+  </si>
+  <si>
+    <t>GPL</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>Apache</t>
+  </si>
+  <si>
+    <t>Subscription</t>
+  </si>
+  <si>
+    <t>The  project is a iOS Mobile App which enables trainers, ambassadors and associates to configure/access/takeup weekly written  quiz, view results of quiz, add a quiz to an Revature Event using the Marketo Code, Allow event attendees to takeup the quiz and  allow trainers to import the questions into RevPro system from their iPhone/iPad devices.</t>
+  </si>
+  <si>
+    <t>As a revature ambassdor I should be able to attach a quiz to an event code.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,13 +440,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -406,6 +450,20 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -610,10 +668,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -625,8 +684,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -646,15 +703,133 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -781,16 +956,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>600904</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>343728</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -818,8 +993,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10629900" y="133351"/>
-          <a:ext cx="1458154" cy="666750"/>
+          <a:off x="9486899" y="504826"/>
+          <a:ext cx="1124779" cy="552449"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -836,14 +1011,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A98B2DB1-16B9-4065-A0C4-86F071896B3D}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A98B2DB1-16B9-4065-A0C4-86F071896B3D}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A1:E20" xr:uid="{738EACD9-D1DD-476D-89AE-BE0A8AD174BA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{48281EE9-E1E6-4DAA-85B7-2708FA1B728D}" name="User Story" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{26A010DA-6018-4309-A586-FC9119BE34A4}" name="Category" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{2BB65B3A-46A4-46ED-AAD1-B5C672623077}" name="Story Points" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{E6656568-54D6-4459-80A3-393D94E9C118}" name="Priority" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{48281EE9-E1E6-4DAA-85B7-2708FA1B728D}" name="User Story" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{26A010DA-6018-4309-A586-FC9119BE34A4}" name="Category" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{2BB65B3A-46A4-46ED-AAD1-B5C672623077}" name="Story Points" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{E6656568-54D6-4459-80A3-393D94E9C118}" name="Priority" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{1F217ECF-B99B-4321-96F4-54D5CE50FBF5}" name="Order"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{800A72FE-978F-4B9B-94C8-13D20F262194}" name="Table2" displayName="Table2" ref="A1:D13" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D13" xr:uid="{28D24CE6-AF33-43C2-A4FC-DB759FF250F3}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{152388AC-42AF-4D8B-84C9-F249F589F787}" name="Technology " dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{7D6F0FC4-3120-4CFF-BDE5-D9D93D28E603}" name="Version" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{3AF1E8E7-A31A-4773-AE09-8FCB9E7541CD}" name="License" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{786607A8-E666-4FC2-955E-1E36BF7BB1B0}" name="Reference" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1146,317 +1334,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B51AEF4D-FF7F-43C0-8915-9F46E5566C6B}">
-  <dimension ref="E8:R24"/>
+  <dimension ref="C2:P19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="30"/>
-    </row>
-    <row r="10" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E10" s="23"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="24"/>
-    </row>
-    <row r="11" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E11" s="23"/>
-      <c r="F11" s="33" t="s">
+    <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="28"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="21"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="22"/>
+    </row>
+    <row r="5" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C5" s="21"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="22"/>
+    </row>
+    <row r="6" spans="3:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="21"/>
+      <c r="D6" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="22"/>
+    </row>
+    <row r="7" spans="3:16" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="21"/>
+      <c r="D7" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="E7" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="22"/>
+    </row>
+    <row r="8" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="21"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="22"/>
+    </row>
+    <row r="9" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C9" s="21"/>
+      <c r="D9" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="24"/>
-    </row>
-    <row r="12" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E12" s="23"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="24"/>
-    </row>
-    <row r="13" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E13" s="23"/>
-      <c r="F13" s="33" t="s">
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="22"/>
+    </row>
+    <row r="10" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="21"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="22"/>
+    </row>
+    <row r="11" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="21"/>
+      <c r="D11" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="35">
+        <v>43892</v>
+      </c>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="22"/>
+    </row>
+    <row r="12" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C12" s="21"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="22"/>
+    </row>
+    <row r="13" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="21"/>
+      <c r="D13" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="E13" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="22"/>
+    </row>
+    <row r="14" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="21"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="22"/>
+    </row>
+    <row r="15" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="21"/>
+      <c r="D15" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="24"/>
-    </row>
-    <row r="14" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E14" s="23"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="24"/>
-    </row>
-    <row r="15" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E15" s="23"/>
-      <c r="F15" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="32" t="s">
+      <c r="E15" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="24"/>
-    </row>
-    <row r="16" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E16" s="23"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="24"/>
-    </row>
-    <row r="17" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E17" s="23"/>
-      <c r="F17" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="34">
-        <v>43892</v>
-      </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="24"/>
-    </row>
-    <row r="18" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E18" s="23"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="24"/>
-    </row>
-    <row r="19" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E19" s="23"/>
-      <c r="F19" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="24"/>
-    </row>
-    <row r="20" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E20" s="23"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="24"/>
-    </row>
-    <row r="21" spans="5:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E21" s="23"/>
-      <c r="F21" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="24"/>
-    </row>
-    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E22" s="23"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="24"/>
-    </row>
-    <row r="23" spans="5:18" x14ac:dyDescent="0.25">
-      <c r="E23" s="23"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="24"/>
-    </row>
-    <row r="24" spans="5:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="27"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="22"/>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C16" s="21"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="22"/>
+    </row>
+    <row r="17" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C17" s="21"/>
+      <c r="D17" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="22"/>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="21"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="22"/>
+    </row>
+    <row r="19" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="25"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E7:N7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E17" r:id="rId1" xr:uid="{61A44AE5-5C45-4B75-9385-B9472C38E7DE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935E299C-709C-43E0-BF4F-FE8920B45D50}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="117.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
@@ -1472,22 +1686,24 @@
         <v>18</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>53</v>
+      <c r="A2" s="33" t="s">
+        <v>52</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1500,9 +1716,11 @@
       <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
       <c r="D3" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -1515,9 +1733,11 @@
       <c r="B4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
       <c r="D4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1527,9 +1747,11 @@
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
       <c r="D5" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,9 +1761,11 @@
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
       <c r="D6" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1551,9 +1775,11 @@
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
       <c r="D7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1563,9 +1789,11 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
       <c r="D8" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1575,9 +1803,11 @@
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
       <c r="D9" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -1590,24 +1820,28 @@
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
       <c r="D10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>46</v>
+      <c r="A11" s="33" t="s">
+        <v>126</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3">
+        <v>5</v>
+      </c>
       <c r="D11" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1620,9 +1854,11 @@
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
       <c r="D12" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -1635,9 +1871,11 @@
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
       <c r="D13" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -1650,9 +1888,11 @@
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
       <c r="D14" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14">
         <v>5</v>
@@ -1665,9 +1905,11 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
       <c r="D15" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -1680,9 +1922,11 @@
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
       <c r="D16" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -1695,9 +1939,11 @@
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
       <c r="D17" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17">
         <v>6</v>
@@ -1705,63 +1951,87 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3">
+        <v>3</v>
+      </c>
       <c r="D18" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>52</v>
+      <c r="A19" s="34" t="s">
+        <v>51</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="9">
+        <v>3</v>
+      </c>
       <c r="D19" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>95</v>
+      <c r="A20" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="9">
+        <v>3</v>
+      </c>
       <c r="D20" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="20">
+        <v>48</v>
+      </c>
+      <c r="E20" s="18">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22">
         <v>14</v>
       </c>
+      <c r="C22">
+        <v>36</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23">
         <v>5</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <f>SUM(Table1[Story Points])</f>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1778,7 +2048,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,24 +2076,27 @@
       <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>92</v>
+      <c r="F1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="13">
         <v>43892</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="13">
         <v>43896</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3">
+        <f>iRevatureQuizPro!$C$22*35/100</f>
+        <v>12.6</v>
+      </c>
       <c r="E2" s="3">
         <f>6*40</f>
         <v>240</v>
@@ -1838,13 +2111,16 @@
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="13">
         <v>43899</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="13">
         <v>43903</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <f>iRevatureQuizPro!$C$22*45/100</f>
+        <v>16.2</v>
+      </c>
       <c r="E3" s="3">
         <f t="shared" ref="E3:E4" si="0">6*40</f>
         <v>240</v>
@@ -1859,13 +2135,16 @@
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="13">
         <v>43906</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>43909</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <f>iRevatureQuizPro!$C$22*20/100</f>
+        <v>7.2</v>
+      </c>
       <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>240</v>
@@ -1880,7 +2159,10 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <f>SUM(D2:D4)</f>
+        <v>36</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1903,27 +2185,27 @@
       <c r="G6" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="1" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1950,21 +2232,21 @@
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>61</v>
+      <c r="B1" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1975,7 +2257,7 @@
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2024,7 +2306,7 @@
         <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2037,7 +2319,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,43 +2335,43 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>93</v>
+        <v>83</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="18">
+      <c r="G2" s="16">
         <v>43895</v>
       </c>
     </row>
@@ -2098,55 +2380,55 @@
         <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="18">
+      <c r="G3" s="16">
         <v>43895</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="18">
+      <c r="G4" s="16">
         <v>43895</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="18">
+      <c r="G5" s="16">
         <v>43895</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>33</v>
@@ -2154,33 +2436,33 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="18">
+      <c r="G6" s="16">
         <v>43894</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>33</v>
@@ -2189,33 +2471,33 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="18">
+      <c r="G8" s="16">
         <v>43899</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="18">
+      <c r="G9" s="16">
         <v>43894</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2233,98 +2515,145 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.140625" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>109</v>
+        <v>104</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="D12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>